<commit_message>
update TestExcel & read data from excel
</commit_message>
<xml_diff>
--- a/testdata/Book1.xlsx
+++ b/testdata/Book1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\IdeaProjects\datadriven\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\IdeaProjects\DataDrivenJava\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>A</t>
   </si>
@@ -48,9 +48,6 @@
   </si>
   <si>
     <t>H</t>
-  </si>
-  <si>
-    <t>HH</t>
   </si>
 </sst>
 </file>
@@ -368,10 +365,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -405,8 +402,27 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
-        <v>8</v>
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>